<commit_message>
Added KKs to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Samuel\workspace\METR4901\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F363A79-37D4-4FD5-9DCC-B4047093B61E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB3B99E-1BDC-4BFB-BBA8-6AD67211772A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9137" windowHeight="0" activeTab="3" xr2:uid="{AF75B441-9CA0-466C-9A03-A4D6E7E2FCD8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9137" windowHeight="0" xr2:uid="{AF75B441-9CA0-466C-9A03-A4D6E7E2FCD8}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="79">
   <si>
     <t>QTY</t>
   </si>
@@ -208,14 +208,76 @@
   </si>
   <si>
     <t>475-1415</t>
+  </si>
+  <si>
+    <t>KK 2 Way</t>
+  </si>
+  <si>
+    <t>KK 3 Way</t>
+  </si>
+  <si>
+    <t>KK 3 Way [Right]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 3 Way, 1 Row, Straight PCB Header, Through Hole </t>
+  </si>
+  <si>
+    <t>483-8477</t>
+  </si>
+  <si>
+    <t>KK 6 way</t>
+  </si>
+  <si>
+    <t>Molex KK 254 6410, 2.54mm Pitch, 6 Way, 1 Row, Straight PCB Header, Through Hole</t>
+  </si>
+  <si>
+    <t>483-8506</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 8 Way, 1 Row, Straight PCB Header, Through Hole </t>
+  </si>
+  <si>
+    <t>KK 8 way</t>
+  </si>
+  <si>
+    <t>483-8528</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 12 Way, 1 Row, Straight PCB Header, Through Hole </t>
+  </si>
+  <si>
+    <t>KK 12 way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 2 Way, 1 Row, Straight PCB Header, Through Hole </t>
+  </si>
+  <si>
+    <t>483-8461</t>
+  </si>
+  <si>
+    <t>Molex KK 254 7478, 2.54mm Pitch, 2 Way, 1 Row, Right Angle PCB Header, Through Hole</t>
+  </si>
+  <si>
+    <t>679-5448</t>
+  </si>
+  <si>
+    <t>483-8540</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Qty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.000_-;\-&quot;$&quot;* #,##0.000_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -259,18 +321,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -301,6 +368,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>234042</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142888</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>87085</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12372</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2531E7A-B978-4A3D-9A7D-4E6886FDA973}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12159342" y="142888"/>
+          <a:ext cx="2639786" cy="4125798"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -600,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD980E25-680F-45CE-A537-9ABE076D869C}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -622,7 +738,7 @@
       </c>
       <c r="E1">
         <f>SUM(E7:E177)</f>
-        <v>0</v>
+        <v>263.76</v>
       </c>
       <c r="K1" t="s">
         <v>36</v>
@@ -640,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q2">
         <v>7</v>
@@ -651,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="Q3">
         <v>26</v>
@@ -707,7 +823,7 @@
       <c r="B7">
         <f>IF(ISERROR(VLOOKUP($A7,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A7,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A7,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A7,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP($A7,Data!$A$2:$D$66,3,FALSE)</f>
@@ -719,7 +835,7 @@
       </c>
       <c r="E7">
         <f>IF(ISERROR(D7*B7),0,D7*B7)</f>
-        <v>0</v>
+        <v>2.8280000000000003</v>
       </c>
       <c r="F7" t="str">
         <f>VLOOKUP($A7,Data!$A$2:$D$66,4,FALSE)</f>
@@ -734,7 +850,10 @@
         <v>3</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3">
+        <f>B7</f>
+        <v>7</v>
+      </c>
       <c r="K7" s="3">
         <f>IF((B7-J7+I7-H7)&lt;0, 0, B7-J7+I7-H7)</f>
         <v>0</v>
@@ -745,7 +864,7 @@
       </c>
       <c r="M7" s="3">
         <f>IF((H7-B7)&lt;0,0,(H7-B7))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
@@ -756,7 +875,7 @@
       <c r="B8">
         <f>IF(ISERROR(VLOOKUP($A8,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A8,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A8,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A8,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP($A8,Data!$A$2:$D$66,3,FALSE)</f>
@@ -768,7 +887,7 @@
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E10" si="0">IF(ISERROR(D8*B8),0,D8*B8)</f>
-        <v>0</v>
+        <v>1.008</v>
       </c>
       <c r="F8" t="str">
         <f>VLOOKUP($A8,Data!$A$2:$D$66,4,FALSE)</f>
@@ -783,18 +902,21 @@
         <v>24</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:J18" si="1">B8</f>
+        <v>28</v>
+      </c>
       <c r="K8" s="3">
-        <f t="shared" ref="K8:K10" si="1">IF((B8-J8+I8-H8)&lt;0, 0, B8-J8+I8-H8)</f>
+        <f t="shared" ref="K8:K10" si="2">IF((B8-J8+I8-H8)&lt;0, 0, B8-J8+I8-H8)</f>
         <v>0</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" ref="L8:L10" si="2">D8*K8</f>
+        <f t="shared" ref="L8:L10" si="3">D8*K8</f>
         <v>0</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" ref="M8:M18" si="3">IF((H8-B8)&lt;0,0,(H8-B8))</f>
-        <v>24</v>
+        <f t="shared" ref="M8:M18" si="4">IF((H8-B8)&lt;0,0,(H8-B8))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
@@ -805,7 +927,7 @@
       <c r="B9">
         <f>IF(ISERROR(VLOOKUP($A9,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A9,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A9,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A9,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP($A9,Data!$A$2:$D$66,3,FALSE)</f>
@@ -817,7 +939,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.008</v>
       </c>
       <c r="F9" t="str">
         <f>VLOOKUP($A9,Data!$A$2:$D$66,4,FALSE)</f>
@@ -832,18 +954,21 @@
         <v>24</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="K9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" si="3"/>
-        <v>24</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
@@ -854,7 +979,7 @@
       <c r="B10">
         <f>IF(ISERROR(VLOOKUP($A10,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A10,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A10,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A10,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C10" t="str">
         <f>VLOOKUP($A10,Data!$A$2:$D$66,3,FALSE)</f>
@@ -866,7 +991,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.252</v>
       </c>
       <c r="F10" t="str">
         <f>VLOOKUP($A10,Data!$A$2:$D$66,4,FALSE)</f>
@@ -881,18 +1006,21 @@
         <v>43</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="K10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" si="3"/>
-        <v>43</v>
+        <f t="shared" si="4"/>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
@@ -903,7 +1031,7 @@
       <c r="B11">
         <f>IF(ISERROR(VLOOKUP($A11,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A11,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A11,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A11,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP($A11,Data!$A$2:$D$66,3,FALSE)</f>
@@ -914,8 +1042,8 @@
         <v>16.73</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11:E18" si="4">IF(ISERROR(D11*B11),0,D11*B11)</f>
-        <v>0</v>
+        <f t="shared" ref="E11:E18" si="5">IF(ISERROR(D11*B11),0,D11*B11)</f>
+        <v>117.11</v>
       </c>
       <c r="F11">
         <f>VLOOKUP($A11,Data!$A$2:$D$66,4,FALSE)</f>
@@ -930,18 +1058,21 @@
         <v>1</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="K11" s="3">
-        <f t="shared" ref="K11:K18" si="5">IF((B11-J11+I11-H11)&lt;0, 0, B11-J11+I11-H11)</f>
+        <f t="shared" ref="K11:K18" si="6">IF((B11-J11+I11-H11)&lt;0, 0, B11-J11+I11-H11)</f>
         <v>0</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" ref="L11:L18" si="6">D11*K11</f>
+        <f t="shared" ref="L11:L18" si="7">D11*K11</f>
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
@@ -952,7 +1083,7 @@
       <c r="B12">
         <f>IF(ISERROR(VLOOKUP($A12,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A12,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A12,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A12,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C12" t="str">
         <f>VLOOKUP($A12,Data!$A$2:$D$66,3,FALSE)</f>
@@ -963,8 +1094,8 @@
         <v>1.3169999999999999</v>
       </c>
       <c r="E12">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>36.875999999999998</v>
       </c>
       <c r="F12">
         <f>VLOOKUP($A12,Data!$A$2:$D$66,4,FALSE)</f>
@@ -979,18 +1110,21 @@
         <v>3</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="J12" s="3">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="K12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
@@ -1001,7 +1135,7 @@
       <c r="B13">
         <f>IF(ISERROR(VLOOKUP($A13,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A13,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A13,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A13,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C13" t="str">
         <f>VLOOKUP($A13,Data!$A$2:$D$66,3,FALSE)</f>
@@ -1012,8 +1146,8 @@
         <v>2.5100000000000002</v>
       </c>
       <c r="E13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>17.57</v>
       </c>
       <c r="F13">
         <f>VLOOKUP($A13,Data!$A$2:$D$66,4,FALSE)</f>
@@ -1028,18 +1162,21 @@
         <v>1</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="J13" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="K13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
@@ -1050,7 +1187,7 @@
       <c r="B14">
         <f>IF(ISERROR(VLOOKUP($A14,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A14,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A14,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A14,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C14" t="str">
         <f>VLOOKUP($A14,Data!$A$2:$D$66,3,FALSE)</f>
@@ -1061,8 +1198,8 @@
         <v>2.8299999999999996</v>
       </c>
       <c r="E14">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>19.809999999999999</v>
       </c>
       <c r="F14">
         <f>VLOOKUP($A14,Data!$A$2:$D$66,4,FALSE)</f>
@@ -1077,18 +1214,21 @@
         <v>1</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="K14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
@@ -1110,7 +1250,7 @@
         <v>1.32</v>
       </c>
       <c r="E15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F15">
@@ -1126,17 +1266,20 @@
         <v>0</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="K15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1159,7 +1302,7 @@
         <v>1.78</v>
       </c>
       <c r="E16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F16">
@@ -1175,21 +1318,24 @@
         <v>0</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="K16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M16" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A17" t="str">
         <f>Data!A12</f>
         <v>PCB Header 45 Pin, Socket</v>
@@ -1208,7 +1354,7 @@
         <v>3.02</v>
       </c>
       <c r="E17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F17">
@@ -1224,21 +1370,24 @@
         <v>0</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="J17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="K17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M17" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" t="str">
         <f>Data!A13</f>
         <v>Ethernet Header</v>
@@ -1246,7 +1395,7 @@
       <c r="B18">
         <f>IF(ISERROR(VLOOKUP($A18,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A18,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
 IF(ISERROR(VLOOKUP($A18,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A18,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" t="str">
         <f>VLOOKUP($A18,Data!$A$2:$D$66,3,FALSE)</f>
@@ -1257,8 +1406,8 @@
         <v>1.8</v>
       </c>
       <c r="E18">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>25.2</v>
       </c>
       <c r="F18">
         <f>VLOOKUP($A18,Data!$A$2:$D$66,4,FALSE)</f>
@@ -1273,23 +1422,762 @@
         <v>2</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="J18" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
       <c r="K18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M18" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A19" t="str">
+        <f>Data!A14</f>
+        <v>Hose Clamp (16mm)</v>
+      </c>
+      <c r="B19">
+        <f>IF(ISERROR(VLOOKUP($A19,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A19,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A19,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A19,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" t="str">
+        <f>VLOOKUP($A19,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>JCS Hi-Torque Steel Slotted Hex Hose Clip Bolt Drive, 9mm Band Width, 14mm - 16mm Inside Diameter</v>
+      </c>
+      <c r="D19">
+        <f>IF(ISERROR(VLOOKUP($A19,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A19,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E30" si="8">IF(ISERROR(D19*B19),0,D19*B19)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" t="str">
+        <f>VLOOKUP($A19,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP($A19,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>727-5936</v>
+      </c>
+      <c r="H19" s="3">
+        <f>Data!F14</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3">
+        <f t="shared" ref="J19:J30" si="9">B19</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" ref="K19:K30" si="10">IF((B19-J19+I19-H19)&lt;0, 0, B19-J19+I19-H19)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" ref="L19:L30" si="11">D19*K19</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" ref="M19:M30" si="12">IF((H19-B19)&lt;0,0,(H19-B19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A20" t="str">
+        <f>Data!A15</f>
+        <v>Nylon Snap Grip</v>
+      </c>
+      <c r="B20">
+        <f>IF(ISERROR(VLOOKUP($A20,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A20,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A20,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A20,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" t="str">
+        <f>VLOOKUP($A20,Data!$A$2:$D$66,3,FALSE)</f>
+        <v xml:space="preserve">RS Pro Nylon Snap Grip, 4.2mm Band Width, 5.6mm - 6.5mm Inside Diameter </v>
+      </c>
+      <c r="D20">
+        <f>IF(ISERROR(VLOOKUP($A20,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A20,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F20" t="str">
+        <f>VLOOKUP($A20,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP($A20,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>475-1415</v>
+      </c>
+      <c r="H20" s="3">
+        <f>Data!F15</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>78</v>
+      </c>
+      <c r="R20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A21" t="str">
+        <f>Data!A16</f>
+        <v>KK 2 Way</v>
+      </c>
+      <c r="B21">
+        <f>IF(ISERROR(VLOOKUP($A21,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A21,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A21,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A21,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" t="str">
+        <f>VLOOKUP($A21,Data!$A$2:$D$66,3,FALSE)</f>
+        <v xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 2 Way, 1 Row, Straight PCB Header, Through Hole </v>
+      </c>
+      <c r="D21">
+        <f>IF(ISERROR(VLOOKUP($A21,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A21,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0.221</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F21" t="str">
+        <f>VLOOKUP($A21,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G21" t="str">
+        <f>VLOOKUP($A21,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>483-8461</v>
+      </c>
+      <c r="H21" s="3">
+        <f>Data!F16</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O21" t="str">
+        <f>A21</f>
+        <v>KK 2 Way</v>
+      </c>
+      <c r="P21" t="str">
+        <f>G21</f>
+        <v>483-8461</v>
+      </c>
+      <c r="Q21" s="6">
+        <f>J21</f>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <f>E21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A22" t="str">
+        <f>Data!A17</f>
+        <v>KK 3 Way</v>
+      </c>
+      <c r="B22">
+        <f>IF(ISERROR(VLOOKUP($A22,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A22,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A22,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A22,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>35</v>
+      </c>
+      <c r="C22" t="str">
+        <f>VLOOKUP($A22,Data!$A$2:$D$66,3,FALSE)</f>
+        <v xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 3 Way, 1 Row, Straight PCB Header, Through Hole </v>
+      </c>
+      <c r="D22">
+        <f>IF(ISERROR(VLOOKUP($A22,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A22,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0.432</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="8"/>
+        <v>15.12</v>
+      </c>
+      <c r="F22" t="str">
+        <f>VLOOKUP($A22,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G22" t="str">
+        <f>VLOOKUP($A22,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>483-8477</v>
+      </c>
+      <c r="H22" s="3">
+        <f>Data!F17</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" ref="O22:O30" si="13">A22</f>
+        <v>KK 3 Way</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" ref="P22:P30" si="14">G22</f>
+        <v>483-8477</v>
+      </c>
+      <c r="Q22" s="6">
+        <f t="shared" ref="Q22:Q30" si="15">J22</f>
+        <v>35</v>
+      </c>
+      <c r="R22">
+        <f t="shared" ref="R22:R26" si="16">E22</f>
+        <v>15.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A23" t="str">
+        <f>Data!A18</f>
+        <v>KK 3 Way [Right]</v>
+      </c>
+      <c r="B23">
+        <f>IF(ISERROR(VLOOKUP($A23,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A23,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A23,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A23,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>28</v>
+      </c>
+      <c r="C23" t="str">
+        <f>VLOOKUP($A23,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>Molex KK 254 7478, 2.54mm Pitch, 2 Way, 1 Row, Right Angle PCB Header, Through Hole</v>
+      </c>
+      <c r="D23">
+        <f>IF(ISERROR(VLOOKUP($A23,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A23,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="8"/>
+        <v>11.06</v>
+      </c>
+      <c r="F23" t="str">
+        <f>VLOOKUP($A23,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G23" t="str">
+        <f>VLOOKUP($A23,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>679-5448</v>
+      </c>
+      <c r="H23" s="3">
+        <f>Data!F18</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="13"/>
+        <v>KK 3 Way [Right]</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="14"/>
+        <v>679-5448</v>
+      </c>
+      <c r="Q23" s="6">
+        <f t="shared" si="15"/>
+        <v>28</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="16"/>
+        <v>11.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A24" t="str">
+        <f>Data!A19</f>
+        <v>KK 6 way</v>
+      </c>
+      <c r="B24">
+        <f>IF(ISERROR(VLOOKUP($A24,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A24,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A24,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A24,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" t="str">
+        <f>VLOOKUP($A24,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>Molex KK 254 6410, 2.54mm Pitch, 6 Way, 1 Row, Straight PCB Header, Through Hole</v>
+      </c>
+      <c r="D24">
+        <f>IF(ISERROR(VLOOKUP($A24,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A24,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F24" t="str">
+        <f>VLOOKUP($A24,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G24" t="str">
+        <f>VLOOKUP($A24,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>483-8506</v>
+      </c>
+      <c r="H24" s="3">
+        <f>Data!F19</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="13"/>
+        <v>KK 6 way</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="14"/>
+        <v>483-8506</v>
+      </c>
+      <c r="Q24" s="6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A25" t="str">
+        <f>Data!A20</f>
+        <v>KK 8 way</v>
+      </c>
+      <c r="B25">
+        <f>IF(ISERROR(VLOOKUP($A25,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A25,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A25,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A25,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" t="str">
+        <f>VLOOKUP($A25,Data!$A$2:$D$66,3,FALSE)</f>
+        <v xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 8 Way, 1 Row, Straight PCB Header, Through Hole </v>
+      </c>
+      <c r="D25">
+        <f>IF(ISERROR(VLOOKUP($A25,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A25,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
+        <f>VLOOKUP($A25,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G25" t="str">
+        <f>VLOOKUP($A25,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>483-8528</v>
+      </c>
+      <c r="H25" s="3">
+        <f>Data!F20</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="13"/>
+        <v>KK 8 way</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="14"/>
+        <v>483-8528</v>
+      </c>
+      <c r="Q25" s="6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A26" t="str">
+        <f>Data!A21</f>
+        <v>KK 12 way</v>
+      </c>
+      <c r="B26">
+        <f>IF(ISERROR(VLOOKUP($A26,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A26,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A26,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A26,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>14</v>
+      </c>
+      <c r="C26" t="str">
+        <f>VLOOKUP($A26,Data!$A$2:$D$66,3,FALSE)</f>
+        <v xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 12 Way, 1 Row, Straight PCB Header, Through Hole </v>
+      </c>
+      <c r="D26">
+        <f>IF(ISERROR(VLOOKUP($A26,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A26,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>1.137</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="8"/>
+        <v>15.917999999999999</v>
+      </c>
+      <c r="F26" t="str">
+        <f>VLOOKUP($A26,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G26" t="str">
+        <f>VLOOKUP($A26,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>483-8540</v>
+      </c>
+      <c r="H26" s="3">
+        <f>Data!F21</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="13"/>
+        <v>KK 12 way</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="14"/>
+        <v>483-8540</v>
+      </c>
+      <c r="Q26" s="6">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="16"/>
+        <v>15.917999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <f>Data!A22</f>
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <f>IF(ISERROR(VLOOKUP($A27,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A27,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A27,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A27,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" t="e">
+        <f>VLOOKUP($A27,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D27">
+        <f>IF(ISERROR(VLOOKUP($A27,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A27,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F27" t="e">
+        <f>VLOOKUP($A27,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G27" t="e">
+        <f>VLOOKUP($A27,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H27" s="3">
+        <f>Data!F22</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <f>Data!A23</f>
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <f>IF(ISERROR(VLOOKUP($A28,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A28,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A28,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A28,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C28" t="e">
+        <f>VLOOKUP($A28,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D28">
+        <f>IF(ISERROR(VLOOKUP($A28,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A28,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F28" t="e">
+        <f>VLOOKUP($A28,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G28" t="e">
+        <f>VLOOKUP($A28,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H28" s="3">
+        <f>Data!F23</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="6"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <f>Data!A24</f>
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <f>IF(ISERROR(VLOOKUP($A29,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A29,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A29,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A29,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" t="e">
+        <f>VLOOKUP($A29,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D29">
+        <f>IF(ISERROR(VLOOKUP($A29,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A29,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F29" t="e">
+        <f>VLOOKUP($A29,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G29" t="e">
+        <f>VLOOKUP($A29,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H29" s="3">
+        <f>Data!F24</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="6"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <f>Data!A25</f>
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <f>IF(ISERROR(VLOOKUP($A30,Mount!$A$2:$F$33,2,FALSE)*$B$2),0,VLOOKUP($A30,Mount!$A$2:$F$33,2,FALSE)*$B$2) +
+IF(ISERROR(VLOOKUP($A30,Sensor!$A$2:$F$33,2,FALSE)*$B$3),0,VLOOKUP($A30,Sensor!$A$2:$F$33,2,FALSE)*$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" t="e">
+        <f>VLOOKUP($A30,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D30">
+        <f>IF(ISERROR(VLOOKUP($A30,Data!$A$2:$D$66,2,FALSE)),0,VLOOKUP($A30,Data!$A$2:$D$66,2,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F30" t="e">
+        <f>VLOOKUP($A30,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G30" t="e">
+        <f>VLOOKUP($A30,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H30" s="3">
+        <f>Data!F25</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:L18" xr:uid="{05399568-C6B0-4EC5-B86A-E9FC6597612F}"/>
-  <conditionalFormatting sqref="K7:K18 O7:O24">
+  <conditionalFormatting sqref="K7:K30 O7:O30">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -1300,10 +2188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FAA6E2-9AD0-48C6-8468-2239704E7287}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1400,9 +2288,6 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4">
-        <v>1.0833333333333333</v>
-      </c>
       <c r="C4" t="str">
         <f>VLOOKUP($A4,Data!$A$2:$D$66,3,FALSE)</f>
         <v>HARWIN M20, 2.54mm Pitch, 36 Way, 1 Row, Straight Pin Header, Through Hole</v>
@@ -1413,7 +2298,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1.43</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f>VLOOKUP($A4,Data!$A$2:$D$66,4,FALSE)</f>
@@ -1428,9 +2313,6 @@
       <c r="A5" t="s">
         <v>51</v>
       </c>
-      <c r="B5">
-        <v>1.1111111111111112</v>
-      </c>
       <c r="C5" t="str">
         <f>VLOOKUP($A5,Data!$A$2:$D$66,3,FALSE)</f>
         <v xml:space="preserve">Stelvio Kontek MODUCOM Series 2.54mm Pitch 45 Way 1 Row Straight PCB Socket, Through Hole, Solder Termination </v>
@@ -1441,7 +2323,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>3.3555555555555556</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f>VLOOKUP($A5,Data!$A$2:$D$66,4,FALSE)</f>
@@ -1562,6 +2444,62 @@
       <c r="G9" t="str">
         <f>VLOOKUP($A9,Data!$A$2:$E$66,5,FALSE)</f>
         <v xml:space="preserve">697-3617 </v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="str">
+        <f>VLOOKUP($A10,Data!$A$2:$D$66,3,FALSE)</f>
+        <v xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 12 Way, 1 Row, Straight PCB Header, Through Hole </v>
+      </c>
+      <c r="D10">
+        <f>VLOOKUP($A10,Data!$A$2:$D$66,2,FALSE)</f>
+        <v>1.137</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E11" si="1">B10*D10</f>
+        <v>2.274</v>
+      </c>
+      <c r="F10" t="str">
+        <f>VLOOKUP($A10,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP($A10,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>483-8540</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="str">
+        <f>VLOOKUP($A11,Data!$A$2:$D$66,3,FALSE)</f>
+        <v xml:space="preserve">Molex KK 254 6410, 2.54mm Pitch, 3 Way, 1 Row, Straight PCB Header, Through Hole </v>
+      </c>
+      <c r="D11">
+        <f>VLOOKUP($A11,Data!$A$2:$D$66,2,FALSE)</f>
+        <v>0.432</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.16</v>
+      </c>
+      <c r="F11" t="str">
+        <f>VLOOKUP($A11,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G11" t="str">
+        <f>VLOOKUP($A11,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>483-8477</v>
       </c>
     </row>
   </sheetData>
@@ -1583,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB523D4-41B9-483E-8DE7-0112CA939A14}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1651,8 +2589,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <f>3/36</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP($A3,Data!$A$2:$D$66,3,FALSE)</f>
@@ -1664,7 +2601,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="0">B3*D3</f>
-        <v>0.14833333333333332</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f>VLOOKUP($A3,Data!$A$2:$D$66,4,FALSE)</f>
@@ -1729,6 +2666,34 @@
       <c r="G5">
         <f>VLOOKUP($A5,Data!$A$2:$E$66,5,FALSE)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP($A6,Data!$A$2:$D$66,3,FALSE)</f>
+        <v>Molex KK 254 7478, 2.54mm Pitch, 2 Way, 1 Row, Right Angle PCB Header, Through Hole</v>
+      </c>
+      <c r="D6">
+        <f>VLOOKUP($A6,Data!$A$2:$D$66,2,FALSE)</f>
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6" si="1">B6*D6</f>
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="F6" t="str">
+        <f>VLOOKUP($A6,Data!$A$2:$D$66,4,FALSE)</f>
+        <v>10 Pack</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP($A6,Data!$A$2:$E$66,5,FALSE)</f>
+        <v>679-5448</v>
       </c>
     </row>
   </sheetData>
@@ -1750,22 +2715,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B80FF8-64CD-4D48-92EC-4974A125A522}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="2" max="2" width="10.78515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="92.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
@@ -1781,11 +2747,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>0.40400000000000003</v>
       </c>
       <c r="C2" t="s">
@@ -1801,11 +2767,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <f>1.8/50</f>
         <v>3.6000000000000004E-2</v>
       </c>
@@ -1822,11 +2788,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <f t="shared" ref="B4:B5" si="0">1.8/50</f>
         <v>3.6000000000000004E-2</v>
       </c>
@@ -1843,11 +2809,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <f t="shared" si="0"/>
         <v>3.6000000000000004E-2</v>
       </c>
@@ -1864,11 +2830,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <f>33.46/2</f>
         <v>16.73</v>
       </c>
@@ -1879,11 +2845,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <f>26.34/20</f>
         <v>1.3169999999999999</v>
       </c>
@@ -1894,11 +2860,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <f>17.57/7</f>
         <v>2.5100000000000002</v>
       </c>
@@ -1909,11 +2875,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <f>19.81/7</f>
         <v>2.8299999999999996</v>
       </c>
@@ -1924,11 +2890,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>1.32</v>
       </c>
       <c r="C10" t="s">
@@ -1938,11 +2904,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>1.78</v>
       </c>
       <c r="C11" t="s">
@@ -1952,11 +2918,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>51</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>3.02</v>
       </c>
       <c r="C12" t="s">
@@ -1966,11 +2932,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>1.8</v>
       </c>
       <c r="C13" t="s">
@@ -1983,11 +2949,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>0.54100000000000004</v>
       </c>
       <c r="C14" t="s">
@@ -2000,11 +2966,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>57</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>0.56200000000000006</v>
       </c>
       <c r="C15" t="s">
@@ -2017,8 +2983,135 @@
         <v>58</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.221</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.432</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1.137</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="G16:G21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>